<commit_message>
Updated with the latest changes
</commit_message>
<xml_diff>
--- a/Lights & Amps.xlsx
+++ b/Lights & Amps.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Code Projects\OrangeJuice\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\IRamp\Code Projects\OrangeJuice\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D0D0648-BBF2-41CD-8FE2-C68D6376770E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62BFE52B-E694-40EE-B92C-54A2580E6C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1116" yWindow="1116" windowWidth="34560" windowHeight="18684" xr2:uid="{BC8B6B45-DEDE-4C80-B1CE-12284D13A983}"/>
+    <workbookView xWindow="1140" yWindow="1140" windowWidth="19300" windowHeight="11250" activeTab="1" xr2:uid="{BC8B6B45-DEDE-4C80-B1CE-12284D13A983}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>Lights</t>
   </si>
@@ -75,6 +76,15 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Ring Light</t>
+  </si>
+  <si>
+    <t>8x8 Matric</t>
+  </si>
+  <si>
+    <t>32x8 Matrix</t>
   </si>
 </sst>
 </file>
@@ -136,7 +146,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2013 - 2022">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -424,7 +434,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme 2013 - 2022" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -434,16 +444,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F0309A42-6DBA-44D4-A25B-324046E311A3}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -457,7 +467,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -472,7 +482,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -487,7 +497,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -502,7 +512,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -517,7 +527,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>5</v>
       </c>
@@ -532,7 +542,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>6</v>
       </c>
@@ -547,7 +557,7 @@
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>7</v>
       </c>
@@ -562,7 +572,7 @@
         <v>4.5</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>8</v>
       </c>
@@ -577,7 +587,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>12</v>
       </c>
@@ -598,4 +608,81 @@
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83A2AA46-0133-47B0-B15F-8DAED7BA183D}">
+  <dimension ref="A1:C5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="10.6328125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2">
+        <v>64</v>
+      </c>
+      <c r="C2">
+        <f>B2*0.06</f>
+        <v>3.84</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3">
+        <v>16</v>
+      </c>
+      <c r="C3">
+        <f t="shared" ref="C3:C5" si="0">B3*0.06</f>
+        <v>0.96</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4">
+        <v>150</v>
+      </c>
+      <c r="C4">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5">
+        <v>256</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>15.36</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>